<commit_message>
Auto-committed on 2021/12/30 週四
Former-commit-id: 81bb3d77bf023a948dda5ef3a9d0fbdc7dfc719a
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/XX-系統/TxFile.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/XX-系統/TxFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="91">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -274,10 +274,6 @@
   </si>
   <si>
     <t>FileDate &gt;= ,AND FileDate &lt;= ,AND BrNo = ,AND CreateEmpNo % ,AND FileCode % ,AND FileItem %</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">FileDate &gt;= ,AND FileDate &lt;= ,AND BrNo = ,AND CreateEmpNo % ,AND FileCode % ,AND FileItem %,AND CreateDate &gt;=,AND CreateDate &lt;  </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -372,6 +368,18 @@
   </si>
   <si>
     <t>CreateDate DESC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>findByFileCodeFirst</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">FileDate &gt;= ,AND FileDate &lt;= ,AND BrNo = ,AND CreateEmpNo % ,AND FileCode % ,AND FileItem %,AND CreateDate &gt;=,AND CreateDate &lt;  </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">FileCode = </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -939,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1012,7 +1020,7 @@
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="15"/>
@@ -1046,22 +1054,22 @@
         <v>0</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="D8" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="E8" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="G8" s="19" t="s">
         <v>69</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1107,7 +1115,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>31</v>
@@ -1130,7 +1138,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>48</v>
@@ -1147,10 +1155,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>35</v>
@@ -1160,7 +1168,7 @@
       </c>
       <c r="F13" s="24"/>
       <c r="G13" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1251,7 +1259,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>60</v>
@@ -1264,7 +1272,7 @@
       </c>
       <c r="F18" s="24"/>
       <c r="G18" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1296,7 +1304,7 @@
         <v>52</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>53</v>
@@ -1333,16 +1341,16 @@
         <v>14</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="E22" s="24" t="s">
         <v>83</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>84</v>
       </c>
       <c r="F22" s="24"/>
       <c r="G22" s="7"/>
@@ -1356,7 +1364,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>13</v>
@@ -1369,7 +1377,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>14</v>
@@ -1433,11 +1441,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1478,7 +1486,7 @@
         <v>63</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1486,25 +1494,86 @@
         <v>62</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="6" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>88</v>
       </c>
+      <c r="B6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>